<commit_message>
Sim Initialization Fully Complete
Proper simulation initialization is complete, only missing part is act method
</commit_message>
<xml_diff>
--- a/Points of Interest.xlsx
+++ b/Points of Interest.xlsx
@@ -210,7 +210,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C5" t="n">
         <v>5.0</v>
@@ -222,7 +222,7 @@
         <v>0.65</v>
       </c>
       <c r="F5" t="n">
-        <v>269.0</v>
+        <v>285.0</v>
       </c>
       <c r="G5" t="n">
         <v>156.0</v>

</xml_diff>